<commit_message>
updated schedule and added task figure
</commit_message>
<xml_diff>
--- a/VisAtten.05_CNRI.xlsx
+++ b/VisAtten.05_CNRI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenna/Library/Mobile Documents/com~apple~CloudDocs/Jenna/duke/CNRI/F23_team/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenna/Documents/CNRIFall23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1853995-3466-304C-98A2-D0A04A5BE7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43EC26B-F765-7941-A54E-37662270B47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5840" yWindow="740" windowWidth="23560" windowHeight="16760" xr2:uid="{DA6A99E7-C06C-2941-B4DD-7875787B3022}"/>
+    <workbookView xWindow="5840" yWindow="740" windowWidth="23560" windowHeight="16760" activeTab="2" xr2:uid="{DA6A99E7-C06C-2941-B4DD-7875787B3022}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -146,15 +146,9 @@
     <t>Week of:</t>
   </si>
   <si>
-    <t>Complete all graphs and figures; Prepare and practice final presentation</t>
-  </si>
-  <si>
     <t>Resource #1</t>
   </si>
   <si>
-    <t>Mediation analyses(?) or partial correlations controlling for age</t>
-  </si>
-  <si>
     <t>Present final presentation</t>
   </si>
   <si>
@@ -170,13 +164,19 @@
     <t>Read and discuss graph theory video; download GitHub</t>
   </si>
   <si>
-    <t>Conduct correlations between age and visual search performance</t>
-  </si>
-  <si>
-    <t>Conduct correlations between age and structural connectivity</t>
-  </si>
-  <si>
-    <t>Draft scatterplots</t>
+    <t>Conduct correlations between age and visual search performance and structural connectivity</t>
+  </si>
+  <si>
+    <t>Plotting correlation and t-test results</t>
+  </si>
+  <si>
+    <t>Conduct partial correlations between search and connectivity, controlling for age</t>
+  </si>
+  <si>
+    <t>Prepare and practice final presentation</t>
+  </si>
+  <si>
+    <t>Complete all graphs and figures</t>
   </si>
 </sst>
 </file>
@@ -736,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A926F14-07B4-1346-BAF3-AC52B24B7984}">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="F64" sqref="F64:I64"/>
     </sheetView>
   </sheetViews>
@@ -747,7 +747,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>0</v>
@@ -2733,8 +2733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E69902E0-97B9-8B49-8E44-090C420FD69B}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2754,7 +2754,7 @@
         <v>10</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>13</v>
@@ -2765,7 +2765,7 @@
         <v>45201</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>17</v>
@@ -2779,7 +2779,7 @@
         <v>45208</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>12</v>
@@ -2793,7 +2793,7 @@
         <v>45215</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>16</v>
@@ -2807,7 +2807,7 @@
         <v>45222</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>18</v>
@@ -2821,7 +2821,7 @@
         <v>45229</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>18</v>
@@ -2835,7 +2835,7 @@
         <v>45236</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>18</v>
@@ -2849,7 +2849,7 @@
         <v>45243</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>18</v>
@@ -2863,7 +2863,7 @@
         <v>45250</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>18</v>
@@ -2877,7 +2877,7 @@
         <v>45257</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>18</v>
@@ -2891,7 +2891,7 @@
         <v>45264</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
modified schedule and readings
</commit_message>
<xml_diff>
--- a/VisAtten.05_CNRI.xlsx
+++ b/VisAtten.05_CNRI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenna/Documents/CNRIFall23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9827C6-6E01-F54E-B88E-E865C2696BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03C4935-E8D0-5749-9D10-8DF95178D27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5840" yWindow="740" windowWidth="23560" windowHeight="16760" activeTab="2" xr2:uid="{DA6A99E7-C06C-2941-B4DD-7875787B3022}"/>
   </bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>age</t>
   </si>
@@ -164,16 +164,37 @@
     <t>Conduct correlations between age and visual search performance and structural connectivity</t>
   </si>
   <si>
-    <t>Conduct partial correlations between search and connectivity, controlling for age</t>
-  </si>
-  <si>
     <t>Prepare and practice final presentation</t>
   </si>
   <si>
     <t>cancelled</t>
   </si>
   <si>
-    <t>Complete all plots: age correlations and t-tests</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ZOOM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>; Read disconnection paper; Complete all plots for age correlations (w/ connectivity and search) and t-tests (between search conditions) by 11/29 meeting</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0306452213009731?via%3Dihub</t>
+  </si>
+  <si>
+    <t>Conduct partial correlations between search and connectivity, controlling for age; continue drafting plots</t>
   </si>
 </sst>
 </file>
@@ -310,7 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -335,7 +356,15 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2743,23 +2772,23 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="52.33203125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="52.33203125" style="19" customWidth="1"/>
     <col min="3" max="3" width="20.5" style="10" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" style="10" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="13" t="s">
@@ -2769,11 +2798,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="15">
         <v>45201</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -2783,11 +2812,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>45208</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="19" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -2797,11 +2826,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <v>45215</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="19" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -2811,11 +2840,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
         <v>45222</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="19" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -2825,11 +2854,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
         <v>45229</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -2839,12 +2868,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <v>45236</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>27</v>
+      <c r="B7" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>18</v>
@@ -2853,26 +2882,26 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
         <v>45243</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>18</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
         <v>45250</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>29</v>
+      <c r="B9" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>18</v>
@@ -2881,12 +2910,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
         <v>45257</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>28</v>
+      <c r="B10" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>18</v>
@@ -2895,11 +2924,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
         <v>45264</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="19" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -2909,11 +2938,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <v>45271</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="19" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="10" t="s">

</xml_diff>